<commit_message>
ext field driven flow
</commit_message>
<xml_diff>
--- a/conversion_algorithm/testing/test.xlsx
+++ b/conversion_algorithm/testing/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justusmulthaup/BA/conversion_algorithm/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A89226-F654-DB45-A137-587DDBADE2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842997DB-E1F7-8D43-A5F7-04347983A330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="500" windowWidth="27680" windowHeight="17500" xr2:uid="{626773B8-1CE5-814C-BDED-1AF936ED64A8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{626773B8-1CE5-814C-BDED-1AF936ED64A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884EA2E4-228E-7348-B965-8C111C291DB8}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,36 +466,50 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>50000</v>
-      </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>1260</v>
-      </c>
-      <c r="D2">
-        <v>115.69</v>
-      </c>
-      <c r="E2" s="2">
-        <v>5.85</v>
-      </c>
-      <c r="F2">
-        <v>648</v>
-      </c>
-      <c r="G2">
-        <f>E2/F2</f>
-        <v>9.0277777777777769E-3</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0.04</v>
-      </c>
+      <c r="E2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>60000</v>
-      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>